<commit_message>
Modificacion del archivo ExcelReader, creacion del archivo ExcelWriter y adaptación del Archivo Excel2Database para añadir las funcionalidades del ExcelWriter
</commit_message>
<xml_diff>
--- a/datos/personas.xlsx
+++ b/datos/personas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t xml:space="preserve">603398467</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOAQUIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOMINGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jdomdom0901@g.educaan.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">640785273</t>
   </si>
 </sst>
 </file>
@@ -176,7 +188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -197,6 +209,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -241,12 +260,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,10 +396,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -568,8 +591,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1" display="jdomdom0901@g.educaan.es"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>